<commit_message>
Os 100 primeiros de Teste
</commit_message>
<xml_diff>
--- a/puma.xlsx
+++ b/puma.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rodrigo Lima\Documents\Cdados\Projeto\projet1cdados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{698FD1A1-40EA-45FC-A416-1C01D8D3B17E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01BF8AD0-E66F-49D4-98A6-528C3885FE76}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Treinamento" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="504">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="504">
   <si>
     <t>Treinamento</t>
   </si>
@@ -2086,8 +2086,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B302"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A290" workbookViewId="0">
-      <selection activeCell="B303" sqref="B303"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4504,568 +4504,874 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:A201"/>
+  <dimension ref="A1:B201"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A159" zoomScale="75" workbookViewId="0">
+      <selection activeCell="B101" sqref="B101"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="140.08984375" customWidth="1"/>
+    <col min="2" max="2" width="23.90625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B1" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>330</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B33" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>340</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>343</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>345</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>350</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>353</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>355</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>358</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>360</v>
       </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>361</v>
       </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>362</v>
       </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>363</v>
       </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>364</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>366</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>370</v>
       </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B70" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>371</v>
       </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>372</v>
       </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>373</v>
       </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>375</v>
       </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>376</v>
       </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>377</v>
       </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>378</v>
       </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>381</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>382</v>
       </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>387</v>
       </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>388</v>
       </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>389</v>
       </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>390</v>
       </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B90">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>391</v>
       </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>392</v>
       </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B93">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>394</v>
       </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>395</v>
       </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>397</v>
       </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>399</v>
       </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>400</v>
       </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B100">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>412</v>
       </c>

</xml_diff>

<commit_message>
separacção de palavras em lista
</commit_message>
<xml_diff>
--- a/puma.xlsx
+++ b/puma.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="202" documentId="13_ncr:1_{01BF8AD0-E66F-49D4-98A6-528C3885FE76}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{3BF15249-5F60-4C03-9AF0-9A25DEA98F53}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Treinamento" sheetId="1" r:id="rId1"/>
@@ -2094,8 +2094,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B301"/>
   <sheetViews>
-    <sheetView topLeftCell="A289" workbookViewId="0">
-      <selection activeCell="D308" sqref="D308"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4521,7 +4521,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A184" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A166" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A200" sqref="A200"/>
     </sheetView>
   </sheetViews>

</xml_diff>